<commit_message>
#26052025: fix change constants null point
</commit_message>
<xml_diff>
--- a/data/CreateCV.xlsx
+++ b/data/CreateCV.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10708"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mac/IdeaProjects/DATNv1/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7594CAD-9DF8-A445-89B1-1757A1A02F81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{A7594CAD-9DF8-A445-89B1-1757A1A02F81}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowHeight="15820" windowWidth="28800" xWindow="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="500"/>
   </bookViews>
   <sheets>
-    <sheet name="data" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="data" r:id="rId1" sheetId="1"/>
+    <sheet name="Sheet1" r:id="rId2" sheetId="2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="49">
   <si>
     <t>Testcase</t>
   </si>
@@ -179,7 +179,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -200,8 +201,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -235,8 +248,18 @@
         <bgColor rgb="FFC00000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125">
+        <bgColor indexed="17"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -397,42 +420,62 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+  <cellXfs count="23">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="1" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="2" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="4" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="3" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="5" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="6" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="7" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="1"/>
+    <xf applyBorder="1" borderId="8" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="1"/>
+    <xf applyFill="1" borderId="0" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="9" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="10" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="11" fillId="5" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="11" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="9" fillId="6" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -449,10 +492,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -487,7 +530,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -522,7 +565,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -616,21 +659,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -647,7 +690,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -699,15 +742,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AD5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AE5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
       <selection activeCell="AA5" sqref="AA5"/>
@@ -715,31 +758,31 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="13.33203125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="32.5" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18.5" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="20.1640625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.83203125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="62.1640625" customWidth="1" collapsed="1"/>
-    <col min="8" max="9" width="12.6640625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="14.6640625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="29.6640625" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="20.33203125" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="20.83203125" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="19.33203125" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="20.5" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="26.5" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="14" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="13.1640625" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="13.5" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="16.83203125" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="22.33203125" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="18.6640625" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="20.5" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="20.1640625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="32.5" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="18.5" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="20.1640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="13.83203125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="62.1640625" collapsed="true"/>
+    <col min="8" max="9" customWidth="true" width="12.6640625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="14.6640625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="29.6640625" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="20.33203125" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="20.83203125" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="19.33203125" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="20.5" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="26.5" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" width="13.1640625" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" width="13.5" collapsed="true"/>
+    <col min="23" max="23" customWidth="true" width="16.83203125" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" width="22.33203125" collapsed="true"/>
+    <col min="25" max="25" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="26" max="26" customWidth="true" width="20.5" collapsed="true"/>
+    <col min="27" max="27" customWidth="true" width="20.1640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row ht="17" r="1" spans="1:30" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
@@ -828,7 +871,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:30" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row ht="16" r="2" spans="1:30" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -849,15 +892,15 @@
       <c r="J2" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="AB2" s="18" t="s">
+      <c r="AB2" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="AC2" s="19" t="s">
+      <c r="AC2" s="22" t="s">
         <v>29</v>
       </c>
       <c r="AD2" s="17"/>
     </row>
-    <row r="3" spans="1:30" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row ht="16" r="3" spans="1:30" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -945,7 +988,7 @@
       </c>
       <c r="AD3" s="15"/>
     </row>
-    <row r="4" spans="1:30" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row ht="16" r="4" spans="1:30" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -967,23 +1010,23 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{0A2BB306-2CB9-4BEE-A991-68A2A40BA9C2}"/>
-    <hyperlink ref="L3" r:id="rId2" xr:uid="{50C9ABE9-837C-4633-A4AF-CB0DAEBFC781}"/>
-    <hyperlink ref="C3" r:id="rId3" xr:uid="{8F3D7588-72BF-3847-A00D-5ECEB8E0AD1D}"/>
+    <hyperlink r:id="rId1" ref="C2" xr:uid="{0A2BB306-2CB9-4BEE-A991-68A2A40BA9C2}"/>
+    <hyperlink r:id="rId2" ref="L3" xr:uid="{50C9ABE9-837C-4633-A4AF-CB0DAEBFC781}"/>
+    <hyperlink r:id="rId3" ref="C3" xr:uid="{8F3D7588-72BF-3847-A00D-5ECEB8E0AD1D}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F78D27F5-8D11-4E77-BAD7-ABAC64DCDE23}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F78D27F5-8D11-4E77-BAD7-ABAC64DCDE23}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>